<commit_message>
Can save a file but still incorrect
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="13995" windowHeight="4905" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="13995" windowHeight="4905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>bar</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -26,11 +26,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sheet2</t>
+    <t>sheet3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sheet3</t>
+    <t>sheet1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -414,8 +418,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>3.3</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -428,35 +464,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
search the cell using format like A2
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -438,6 +438,11 @@
       </c>
       <c r="B2">
         <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.15">
+      <c r="H27">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>